<commit_message>
Some work for clearing code
</commit_message>
<xml_diff>
--- a/Neural Network for Finance/BTCUSDTDCHG.xlsx
+++ b/Neural Network for Finance/BTCUSDTDCHG.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1819"/>
+  <dimension ref="A1:I1886"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,18 +500,10 @@
       <c r="E2" t="n">
         <v>4285.08</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -529,18 +521,10 @@
       <c r="E3" t="n">
         <v>4108.37</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -558,18 +542,10 @@
       <c r="E4" t="n">
         <v>4139.98</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -587,18 +563,10 @@
       <c r="E5" t="n">
         <v>4086.29</v>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -616,18 +584,10 @@
       <c r="E6" t="n">
         <v>4016</v>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -645,18 +605,10 @@
       <c r="E7" t="n">
         <v>4040</v>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -53191,7 +53143,7 @@
         <v>23154.25</v>
       </c>
       <c r="E1819" t="n">
-        <v>23953.58</v>
+        <v>23810</v>
       </c>
       <c r="F1819" t="n">
         <v>23266.9</v>
@@ -53204,6 +53156,1949 @@
       </c>
       <c r="I1819" t="n">
         <v>22987.79</v>
+      </c>
+    </row>
+    <row r="1820">
+      <c r="A1820" s="2" t="n">
+        <v>44782</v>
+      </c>
+      <c r="B1820" t="n">
+        <v>23810.98</v>
+      </c>
+      <c r="C1820" t="n">
+        <v>23933.25</v>
+      </c>
+      <c r="D1820" t="n">
+        <v>22865</v>
+      </c>
+      <c r="E1820" t="n">
+        <v>23149.95</v>
+      </c>
+      <c r="F1820" t="n">
+        <v>22985.93</v>
+      </c>
+      <c r="G1820" t="n">
+        <v>24245</v>
+      </c>
+      <c r="H1820" t="n">
+        <v>22400</v>
+      </c>
+      <c r="I1820" t="n">
+        <v>22818.37</v>
+      </c>
+    </row>
+    <row r="1821">
+      <c r="A1821" s="2" t="n">
+        <v>44783</v>
+      </c>
+      <c r="B1821" t="n">
+        <v>23151.32</v>
+      </c>
+      <c r="C1821" t="n">
+        <v>24226</v>
+      </c>
+      <c r="D1821" t="n">
+        <v>22664.69</v>
+      </c>
+      <c r="E1821" t="n">
+        <v>23954.05</v>
+      </c>
+      <c r="F1821" t="n">
+        <v>22816.91</v>
+      </c>
+      <c r="G1821" t="n">
+        <v>24245</v>
+      </c>
+      <c r="H1821" t="n">
+        <v>22400</v>
+      </c>
+      <c r="I1821" t="n">
+        <v>22622.98</v>
+      </c>
+    </row>
+    <row r="1822">
+      <c r="A1822" s="2" t="n">
+        <v>44784</v>
+      </c>
+      <c r="B1822" t="n">
+        <v>23954.05</v>
+      </c>
+      <c r="C1822" t="n">
+        <v>24918.54</v>
+      </c>
+      <c r="D1822" t="n">
+        <v>23852.13</v>
+      </c>
+      <c r="E1822" t="n">
+        <v>23934.39</v>
+      </c>
+      <c r="F1822" t="n">
+        <v>22622.41</v>
+      </c>
+      <c r="G1822" t="n">
+        <v>24918.54</v>
+      </c>
+      <c r="H1822" t="n">
+        <v>22586.95</v>
+      </c>
+      <c r="I1822" t="n">
+        <v>23312.42</v>
+      </c>
+    </row>
+    <row r="1823">
+      <c r="A1823" s="2" t="n">
+        <v>44785</v>
+      </c>
+      <c r="B1823" t="n">
+        <v>23933.09</v>
+      </c>
+      <c r="C1823" t="n">
+        <v>24456.5</v>
+      </c>
+      <c r="D1823" t="n">
+        <v>23583</v>
+      </c>
+      <c r="E1823" t="n">
+        <v>24403.68</v>
+      </c>
+      <c r="F1823" t="n">
+        <v>23313.56</v>
+      </c>
+      <c r="G1823" t="n">
+        <v>24918.54</v>
+      </c>
+      <c r="H1823" t="n">
+        <v>22664.69</v>
+      </c>
+      <c r="I1823" t="n">
+        <v>22954.21</v>
+      </c>
+    </row>
+    <row r="1824">
+      <c r="A1824" s="2" t="n">
+        <v>44786</v>
+      </c>
+      <c r="B1824" t="n">
+        <v>24401.7</v>
+      </c>
+      <c r="C1824" t="n">
+        <v>24888</v>
+      </c>
+      <c r="D1824" t="n">
+        <v>24291.22</v>
+      </c>
+      <c r="E1824" t="n">
+        <v>24441.38</v>
+      </c>
+      <c r="F1824" t="n">
+        <v>22954.21</v>
+      </c>
+      <c r="G1824" t="n">
+        <v>24918.54</v>
+      </c>
+      <c r="H1824" t="n">
+        <v>22664.69</v>
+      </c>
+      <c r="I1824" t="n">
+        <v>23174.39</v>
+      </c>
+    </row>
+    <row r="1825">
+      <c r="A1825" s="2" t="n">
+        <v>44787</v>
+      </c>
+      <c r="B1825" t="n">
+        <v>24443.06</v>
+      </c>
+      <c r="C1825" t="n">
+        <v>25047.56</v>
+      </c>
+      <c r="D1825" t="n">
+        <v>24144</v>
+      </c>
+      <c r="E1825" t="n">
+        <v>24305.24</v>
+      </c>
+      <c r="F1825" t="n">
+        <v>23174.39</v>
+      </c>
+      <c r="G1825" t="n">
+        <v>25047.56</v>
+      </c>
+      <c r="H1825" t="n">
+        <v>22664.69</v>
+      </c>
+      <c r="I1825" t="n">
+        <v>23810</v>
+      </c>
+    </row>
+    <row r="1826">
+      <c r="A1826" s="2" t="n">
+        <v>44788</v>
+      </c>
+      <c r="B1826" t="n">
+        <v>24305.25</v>
+      </c>
+      <c r="C1826" t="n">
+        <v>25211.32</v>
+      </c>
+      <c r="D1826" t="n">
+        <v>23773.22</v>
+      </c>
+      <c r="E1826" t="n">
+        <v>24094.82</v>
+      </c>
+      <c r="F1826" t="n">
+        <v>23810.98</v>
+      </c>
+      <c r="G1826" t="n">
+        <v>25211.32</v>
+      </c>
+      <c r="H1826" t="n">
+        <v>22664.69</v>
+      </c>
+      <c r="I1826" t="n">
+        <v>23149.95</v>
+      </c>
+    </row>
+    <row r="1827">
+      <c r="A1827" s="2" t="n">
+        <v>44789</v>
+      </c>
+      <c r="B1827" t="n">
+        <v>24093.04</v>
+      </c>
+      <c r="C1827" t="n">
+        <v>24247.49</v>
+      </c>
+      <c r="D1827" t="n">
+        <v>23671.22</v>
+      </c>
+      <c r="E1827" t="n">
+        <v>23854.74</v>
+      </c>
+      <c r="F1827" t="n">
+        <v>23151.32</v>
+      </c>
+      <c r="G1827" t="n">
+        <v>25211.32</v>
+      </c>
+      <c r="H1827" t="n">
+        <v>22664.69</v>
+      </c>
+      <c r="I1827" t="n">
+        <v>23954.05</v>
+      </c>
+    </row>
+    <row r="1828">
+      <c r="A1828" s="2" t="n">
+        <v>44790</v>
+      </c>
+      <c r="B1828" t="n">
+        <v>23856.15</v>
+      </c>
+      <c r="C1828" t="n">
+        <v>24446.71</v>
+      </c>
+      <c r="D1828" t="n">
+        <v>23180.4</v>
+      </c>
+      <c r="E1828" t="n">
+        <v>23342.66</v>
+      </c>
+      <c r="F1828" t="n">
+        <v>23954.05</v>
+      </c>
+      <c r="G1828" t="n">
+        <v>25211.32</v>
+      </c>
+      <c r="H1828" t="n">
+        <v>23180.4</v>
+      </c>
+      <c r="I1828" t="n">
+        <v>23934.39</v>
+      </c>
+    </row>
+    <row r="1829">
+      <c r="A1829" s="2" t="n">
+        <v>44791</v>
+      </c>
+      <c r="B1829" t="n">
+        <v>23342.66</v>
+      </c>
+      <c r="C1829" t="n">
+        <v>23600</v>
+      </c>
+      <c r="D1829" t="n">
+        <v>23111.04</v>
+      </c>
+      <c r="E1829" t="n">
+        <v>23191.2</v>
+      </c>
+      <c r="F1829" t="n">
+        <v>23933.09</v>
+      </c>
+      <c r="G1829" t="n">
+        <v>25211.32</v>
+      </c>
+      <c r="H1829" t="n">
+        <v>23111.04</v>
+      </c>
+      <c r="I1829" t="n">
+        <v>24403.68</v>
+      </c>
+    </row>
+    <row r="1830">
+      <c r="A1830" s="2" t="n">
+        <v>44792</v>
+      </c>
+      <c r="B1830" t="n">
+        <v>23191.45</v>
+      </c>
+      <c r="C1830" t="n">
+        <v>23208.67</v>
+      </c>
+      <c r="D1830" t="n">
+        <v>20783.57</v>
+      </c>
+      <c r="E1830" t="n">
+        <v>20834.39</v>
+      </c>
+      <c r="F1830" t="n">
+        <v>24401.7</v>
+      </c>
+      <c r="G1830" t="n">
+        <v>25211.32</v>
+      </c>
+      <c r="H1830" t="n">
+        <v>20783.57</v>
+      </c>
+      <c r="I1830" t="n">
+        <v>24441.38</v>
+      </c>
+    </row>
+    <row r="1831">
+      <c r="A1831" s="2" t="n">
+        <v>44793</v>
+      </c>
+      <c r="B1831" t="n">
+        <v>20834.39</v>
+      </c>
+      <c r="C1831" t="n">
+        <v>21382.85</v>
+      </c>
+      <c r="D1831" t="n">
+        <v>20761.9</v>
+      </c>
+      <c r="E1831" t="n">
+        <v>21140.07</v>
+      </c>
+      <c r="F1831" t="n">
+        <v>24443.06</v>
+      </c>
+      <c r="G1831" t="n">
+        <v>25211.32</v>
+      </c>
+      <c r="H1831" t="n">
+        <v>20761.9</v>
+      </c>
+      <c r="I1831" t="n">
+        <v>24305.24</v>
+      </c>
+    </row>
+    <row r="1832">
+      <c r="A1832" s="2" t="n">
+        <v>44794</v>
+      </c>
+      <c r="B1832" t="n">
+        <v>21140.07</v>
+      </c>
+      <c r="C1832" t="n">
+        <v>21800</v>
+      </c>
+      <c r="D1832" t="n">
+        <v>21069.11</v>
+      </c>
+      <c r="E1832" t="n">
+        <v>21515.61</v>
+      </c>
+      <c r="F1832" t="n">
+        <v>24305.25</v>
+      </c>
+      <c r="G1832" t="n">
+        <v>25211.32</v>
+      </c>
+      <c r="H1832" t="n">
+        <v>20761.9</v>
+      </c>
+      <c r="I1832" t="n">
+        <v>24094.82</v>
+      </c>
+    </row>
+    <row r="1833">
+      <c r="A1833" s="2" t="n">
+        <v>44795</v>
+      </c>
+      <c r="B1833" t="n">
+        <v>21516.7</v>
+      </c>
+      <c r="C1833" t="n">
+        <v>21548.71</v>
+      </c>
+      <c r="D1833" t="n">
+        <v>20890.18</v>
+      </c>
+      <c r="E1833" t="n">
+        <v>21399.83</v>
+      </c>
+      <c r="F1833" t="n">
+        <v>24093.04</v>
+      </c>
+      <c r="G1833" t="n">
+        <v>24446.71</v>
+      </c>
+      <c r="H1833" t="n">
+        <v>20761.9</v>
+      </c>
+      <c r="I1833" t="n">
+        <v>23854.74</v>
+      </c>
+    </row>
+    <row r="1834">
+      <c r="A1834" s="2" t="n">
+        <v>44796</v>
+      </c>
+      <c r="B1834" t="n">
+        <v>21400.75</v>
+      </c>
+      <c r="C1834" t="n">
+        <v>21684.87</v>
+      </c>
+      <c r="D1834" t="n">
+        <v>20890.14</v>
+      </c>
+      <c r="E1834" t="n">
+        <v>21529.12</v>
+      </c>
+      <c r="F1834" t="n">
+        <v>23856.15</v>
+      </c>
+      <c r="G1834" t="n">
+        <v>24446.71</v>
+      </c>
+      <c r="H1834" t="n">
+        <v>20761.9</v>
+      </c>
+      <c r="I1834" t="n">
+        <v>23342.66</v>
+      </c>
+    </row>
+    <row r="1835">
+      <c r="A1835" s="2" t="n">
+        <v>44797</v>
+      </c>
+      <c r="B1835" t="n">
+        <v>21529.11</v>
+      </c>
+      <c r="C1835" t="n">
+        <v>21900</v>
+      </c>
+      <c r="D1835" t="n">
+        <v>21145</v>
+      </c>
+      <c r="E1835" t="n">
+        <v>21368.08</v>
+      </c>
+      <c r="F1835" t="n">
+        <v>23342.66</v>
+      </c>
+      <c r="G1835" t="n">
+        <v>23600</v>
+      </c>
+      <c r="H1835" t="n">
+        <v>20761.9</v>
+      </c>
+      <c r="I1835" t="n">
+        <v>23191.2</v>
+      </c>
+    </row>
+    <row r="1836">
+      <c r="A1836" s="2" t="n">
+        <v>44798</v>
+      </c>
+      <c r="B1836" t="n">
+        <v>21368.05</v>
+      </c>
+      <c r="C1836" t="n">
+        <v>21819.88</v>
+      </c>
+      <c r="D1836" t="n">
+        <v>21310.15</v>
+      </c>
+      <c r="E1836" t="n">
+        <v>21559.04</v>
+      </c>
+      <c r="F1836" t="n">
+        <v>23191.45</v>
+      </c>
+      <c r="G1836" t="n">
+        <v>23208.67</v>
+      </c>
+      <c r="H1836" t="n">
+        <v>20761.9</v>
+      </c>
+      <c r="I1836" t="n">
+        <v>20834.39</v>
+      </c>
+    </row>
+    <row r="1837">
+      <c r="A1837" s="2" t="n">
+        <v>44799</v>
+      </c>
+      <c r="B1837" t="n">
+        <v>21559.04</v>
+      </c>
+      <c r="C1837" t="n">
+        <v>21886.77</v>
+      </c>
+      <c r="D1837" t="n">
+        <v>20107.9</v>
+      </c>
+      <c r="E1837" t="n">
+        <v>20241.05</v>
+      </c>
+      <c r="F1837" t="n">
+        <v>20834.39</v>
+      </c>
+      <c r="G1837" t="n">
+        <v>21900</v>
+      </c>
+      <c r="H1837" t="n">
+        <v>20107.9</v>
+      </c>
+      <c r="I1837" t="n">
+        <v>21140.07</v>
+      </c>
+    </row>
+    <row r="1838">
+      <c r="A1838" s="2" t="n">
+        <v>44800</v>
+      </c>
+      <c r="B1838" t="n">
+        <v>20239.14</v>
+      </c>
+      <c r="C1838" t="n">
+        <v>20402.93</v>
+      </c>
+      <c r="D1838" t="n">
+        <v>19800</v>
+      </c>
+      <c r="E1838" t="n">
+        <v>20037.6</v>
+      </c>
+      <c r="F1838" t="n">
+        <v>21140.07</v>
+      </c>
+      <c r="G1838" t="n">
+        <v>21900</v>
+      </c>
+      <c r="H1838" t="n">
+        <v>19800</v>
+      </c>
+      <c r="I1838" t="n">
+        <v>21515.61</v>
+      </c>
+    </row>
+    <row r="1839">
+      <c r="A1839" s="2" t="n">
+        <v>44801</v>
+      </c>
+      <c r="B1839" t="n">
+        <v>20037.6</v>
+      </c>
+      <c r="C1839" t="n">
+        <v>20171.18</v>
+      </c>
+      <c r="D1839" t="n">
+        <v>19520</v>
+      </c>
+      <c r="E1839" t="n">
+        <v>19555.61</v>
+      </c>
+      <c r="F1839" t="n">
+        <v>21516.7</v>
+      </c>
+      <c r="G1839" t="n">
+        <v>21900</v>
+      </c>
+      <c r="H1839" t="n">
+        <v>19520</v>
+      </c>
+      <c r="I1839" t="n">
+        <v>21399.83</v>
+      </c>
+    </row>
+    <row r="1840">
+      <c r="A1840" s="2" t="n">
+        <v>44802</v>
+      </c>
+      <c r="B1840" t="n">
+        <v>19555.61</v>
+      </c>
+      <c r="C1840" t="n">
+        <v>20433.62</v>
+      </c>
+      <c r="D1840" t="n">
+        <v>19550.79</v>
+      </c>
+      <c r="E1840" t="n">
+        <v>20285.73</v>
+      </c>
+      <c r="F1840" t="n">
+        <v>21400.75</v>
+      </c>
+      <c r="G1840" t="n">
+        <v>21900</v>
+      </c>
+      <c r="H1840" t="n">
+        <v>19520</v>
+      </c>
+      <c r="I1840" t="n">
+        <v>21529.12</v>
+      </c>
+    </row>
+    <row r="1841">
+      <c r="A1841" s="2" t="n">
+        <v>44803</v>
+      </c>
+      <c r="B1841" t="n">
+        <v>20287.2</v>
+      </c>
+      <c r="C1841" t="n">
+        <v>20576.25</v>
+      </c>
+      <c r="D1841" t="n">
+        <v>19540</v>
+      </c>
+      <c r="E1841" t="n">
+        <v>19811.66</v>
+      </c>
+      <c r="F1841" t="n">
+        <v>21529.11</v>
+      </c>
+      <c r="G1841" t="n">
+        <v>21900</v>
+      </c>
+      <c r="H1841" t="n">
+        <v>19520</v>
+      </c>
+      <c r="I1841" t="n">
+        <v>21368.08</v>
+      </c>
+    </row>
+    <row r="1842">
+      <c r="A1842" s="2" t="n">
+        <v>44804</v>
+      </c>
+      <c r="B1842" t="n">
+        <v>19813.03</v>
+      </c>
+      <c r="C1842" t="n">
+        <v>20490</v>
+      </c>
+      <c r="D1842" t="n">
+        <v>19797.94</v>
+      </c>
+      <c r="E1842" t="n">
+        <v>20050.02</v>
+      </c>
+      <c r="F1842" t="n">
+        <v>21368.05</v>
+      </c>
+      <c r="G1842" t="n">
+        <v>21886.77</v>
+      </c>
+      <c r="H1842" t="n">
+        <v>19520</v>
+      </c>
+      <c r="I1842" t="n">
+        <v>21559.04</v>
+      </c>
+    </row>
+    <row r="1843">
+      <c r="A1843" s="2" t="n">
+        <v>44805</v>
+      </c>
+      <c r="B1843" t="n">
+        <v>20048.44</v>
+      </c>
+      <c r="C1843" t="n">
+        <v>20208.37</v>
+      </c>
+      <c r="D1843" t="n">
+        <v>19565.66</v>
+      </c>
+      <c r="E1843" t="n">
+        <v>20131.46</v>
+      </c>
+      <c r="F1843" t="n">
+        <v>21559.04</v>
+      </c>
+      <c r="G1843" t="n">
+        <v>21886.77</v>
+      </c>
+      <c r="H1843" t="n">
+        <v>19520</v>
+      </c>
+      <c r="I1843" t="n">
+        <v>20241.05</v>
+      </c>
+    </row>
+    <row r="1844">
+      <c r="A1844" s="2" t="n">
+        <v>44806</v>
+      </c>
+      <c r="B1844" t="n">
+        <v>20132.64</v>
+      </c>
+      <c r="C1844" t="n">
+        <v>20441.26</v>
+      </c>
+      <c r="D1844" t="n">
+        <v>19755.29</v>
+      </c>
+      <c r="E1844" t="n">
+        <v>19951.86</v>
+      </c>
+      <c r="F1844" t="n">
+        <v>20239.14</v>
+      </c>
+      <c r="G1844" t="n">
+        <v>20576.25</v>
+      </c>
+      <c r="H1844" t="n">
+        <v>19520</v>
+      </c>
+      <c r="I1844" t="n">
+        <v>20037.6</v>
+      </c>
+    </row>
+    <row r="1845">
+      <c r="A1845" s="2" t="n">
+        <v>44807</v>
+      </c>
+      <c r="B1845" t="n">
+        <v>19950.98</v>
+      </c>
+      <c r="C1845" t="n">
+        <v>20055.93</v>
+      </c>
+      <c r="D1845" t="n">
+        <v>19652.72</v>
+      </c>
+      <c r="E1845" t="n">
+        <v>19831.9</v>
+      </c>
+      <c r="F1845" t="n">
+        <v>20037.6</v>
+      </c>
+      <c r="G1845" t="n">
+        <v>20576.25</v>
+      </c>
+      <c r="H1845" t="n">
+        <v>19520</v>
+      </c>
+      <c r="I1845" t="n">
+        <v>19555.61</v>
+      </c>
+    </row>
+    <row r="1846">
+      <c r="A1846" s="2" t="n">
+        <v>44808</v>
+      </c>
+      <c r="B1846" t="n">
+        <v>19832.45</v>
+      </c>
+      <c r="C1846" t="n">
+        <v>20029.23</v>
+      </c>
+      <c r="D1846" t="n">
+        <v>19583.1</v>
+      </c>
+      <c r="E1846" t="n">
+        <v>20000.3</v>
+      </c>
+      <c r="F1846" t="n">
+        <v>19555.61</v>
+      </c>
+      <c r="G1846" t="n">
+        <v>20576.25</v>
+      </c>
+      <c r="H1846" t="n">
+        <v>19540</v>
+      </c>
+      <c r="I1846" t="n">
+        <v>20285.73</v>
+      </c>
+    </row>
+    <row r="1847">
+      <c r="A1847" s="2" t="n">
+        <v>44809</v>
+      </c>
+      <c r="B1847" t="n">
+        <v>20000.3</v>
+      </c>
+      <c r="C1847" t="n">
+        <v>20057.27</v>
+      </c>
+      <c r="D1847" t="n">
+        <v>19633.83</v>
+      </c>
+      <c r="E1847" t="n">
+        <v>19796.84</v>
+      </c>
+      <c r="F1847" t="n">
+        <v>20287.2</v>
+      </c>
+      <c r="G1847" t="n">
+        <v>20576.25</v>
+      </c>
+      <c r="H1847" t="n">
+        <v>19540</v>
+      </c>
+      <c r="I1847" t="n">
+        <v>19811.66</v>
+      </c>
+    </row>
+    <row r="1848">
+      <c r="A1848" s="2" t="n">
+        <v>44810</v>
+      </c>
+      <c r="B1848" t="n">
+        <v>19795.34</v>
+      </c>
+      <c r="C1848" t="n">
+        <v>20180</v>
+      </c>
+      <c r="D1848" t="n">
+        <v>18649.51</v>
+      </c>
+      <c r="E1848" t="n">
+        <v>18790.61</v>
+      </c>
+      <c r="F1848" t="n">
+        <v>19813.03</v>
+      </c>
+      <c r="G1848" t="n">
+        <v>20490</v>
+      </c>
+      <c r="H1848" t="n">
+        <v>18649.51</v>
+      </c>
+      <c r="I1848" t="n">
+        <v>20050.02</v>
+      </c>
+    </row>
+    <row r="1849">
+      <c r="A1849" s="2" t="n">
+        <v>44811</v>
+      </c>
+      <c r="B1849" t="n">
+        <v>18790.61</v>
+      </c>
+      <c r="C1849" t="n">
+        <v>19464.06</v>
+      </c>
+      <c r="D1849" t="n">
+        <v>18510.77</v>
+      </c>
+      <c r="E1849" t="n">
+        <v>19292.84</v>
+      </c>
+      <c r="F1849" t="n">
+        <v>20048.44</v>
+      </c>
+      <c r="G1849" t="n">
+        <v>20441.26</v>
+      </c>
+      <c r="H1849" t="n">
+        <v>18510.77</v>
+      </c>
+      <c r="I1849" t="n">
+        <v>20131.46</v>
+      </c>
+    </row>
+    <row r="1850">
+      <c r="A1850" s="2" t="n">
+        <v>44812</v>
+      </c>
+      <c r="B1850" t="n">
+        <v>19292.85</v>
+      </c>
+      <c r="C1850" t="n">
+        <v>19458.25</v>
+      </c>
+      <c r="D1850" t="n">
+        <v>19012</v>
+      </c>
+      <c r="E1850" t="n">
+        <v>19319.77</v>
+      </c>
+      <c r="F1850" t="n">
+        <v>20132.64</v>
+      </c>
+      <c r="G1850" t="n">
+        <v>20441.26</v>
+      </c>
+      <c r="H1850" t="n">
+        <v>18510.77</v>
+      </c>
+      <c r="I1850" t="n">
+        <v>19951.86</v>
+      </c>
+    </row>
+    <row r="1851">
+      <c r="A1851" s="2" t="n">
+        <v>44813</v>
+      </c>
+      <c r="B1851" t="n">
+        <v>19320.54</v>
+      </c>
+      <c r="C1851" t="n">
+        <v>21597.22</v>
+      </c>
+      <c r="D1851" t="n">
+        <v>19291.75</v>
+      </c>
+      <c r="E1851" t="n">
+        <v>21360.11</v>
+      </c>
+      <c r="F1851" t="n">
+        <v>19950.98</v>
+      </c>
+      <c r="G1851" t="n">
+        <v>21597.22</v>
+      </c>
+      <c r="H1851" t="n">
+        <v>18510.77</v>
+      </c>
+      <c r="I1851" t="n">
+        <v>19831.9</v>
+      </c>
+    </row>
+    <row r="1852">
+      <c r="A1852" s="2" t="n">
+        <v>44814</v>
+      </c>
+      <c r="B1852" t="n">
+        <v>21361.62</v>
+      </c>
+      <c r="C1852" t="n">
+        <v>21810.8</v>
+      </c>
+      <c r="D1852" t="n">
+        <v>21111.13</v>
+      </c>
+      <c r="E1852" t="n">
+        <v>21648.34</v>
+      </c>
+      <c r="F1852" t="n">
+        <v>19832.45</v>
+      </c>
+      <c r="G1852" t="n">
+        <v>21810.8</v>
+      </c>
+      <c r="H1852" t="n">
+        <v>18510.77</v>
+      </c>
+      <c r="I1852" t="n">
+        <v>20000.3</v>
+      </c>
+    </row>
+    <row r="1853">
+      <c r="A1853" s="2" t="n">
+        <v>44815</v>
+      </c>
+      <c r="B1853" t="n">
+        <v>21647.21</v>
+      </c>
+      <c r="C1853" t="n">
+        <v>21860</v>
+      </c>
+      <c r="D1853" t="n">
+        <v>21350</v>
+      </c>
+      <c r="E1853" t="n">
+        <v>21826.87</v>
+      </c>
+      <c r="F1853" t="n">
+        <v>20000.3</v>
+      </c>
+      <c r="G1853" t="n">
+        <v>21860</v>
+      </c>
+      <c r="H1853" t="n">
+        <v>18510.77</v>
+      </c>
+      <c r="I1853" t="n">
+        <v>19796.84</v>
+      </c>
+    </row>
+    <row r="1854">
+      <c r="A1854" s="2" t="n">
+        <v>44816</v>
+      </c>
+      <c r="B1854" t="n">
+        <v>21826.87</v>
+      </c>
+      <c r="C1854" t="n">
+        <v>22488</v>
+      </c>
+      <c r="D1854" t="n">
+        <v>21538.51</v>
+      </c>
+      <c r="E1854" t="n">
+        <v>22395.74</v>
+      </c>
+      <c r="F1854" t="n">
+        <v>19795.34</v>
+      </c>
+      <c r="G1854" t="n">
+        <v>22488</v>
+      </c>
+      <c r="H1854" t="n">
+        <v>18510.77</v>
+      </c>
+      <c r="I1854" t="n">
+        <v>18790.61</v>
+      </c>
+    </row>
+    <row r="1855">
+      <c r="A1855" s="2" t="n">
+        <v>44817</v>
+      </c>
+      <c r="B1855" t="n">
+        <v>22395.44</v>
+      </c>
+      <c r="C1855" t="n">
+        <v>22799</v>
+      </c>
+      <c r="D1855" t="n">
+        <v>19860</v>
+      </c>
+      <c r="E1855" t="n">
+        <v>20173.57</v>
+      </c>
+      <c r="F1855" t="n">
+        <v>18790.61</v>
+      </c>
+      <c r="G1855" t="n">
+        <v>22799</v>
+      </c>
+      <c r="H1855" t="n">
+        <v>18510.77</v>
+      </c>
+      <c r="I1855" t="n">
+        <v>19292.84</v>
+      </c>
+    </row>
+    <row r="1856">
+      <c r="A1856" s="2" t="n">
+        <v>44818</v>
+      </c>
+      <c r="B1856" t="n">
+        <v>20173.62</v>
+      </c>
+      <c r="C1856" t="n">
+        <v>20541.48</v>
+      </c>
+      <c r="D1856" t="n">
+        <v>19617.62</v>
+      </c>
+      <c r="E1856" t="n">
+        <v>20226.71</v>
+      </c>
+      <c r="F1856" t="n">
+        <v>19292.85</v>
+      </c>
+      <c r="G1856" t="n">
+        <v>22799</v>
+      </c>
+      <c r="H1856" t="n">
+        <v>19012</v>
+      </c>
+      <c r="I1856" t="n">
+        <v>19319.77</v>
+      </c>
+    </row>
+    <row r="1857">
+      <c r="A1857" s="2" t="n">
+        <v>44819</v>
+      </c>
+      <c r="B1857" t="n">
+        <v>20227.17</v>
+      </c>
+      <c r="C1857" t="n">
+        <v>20330.24</v>
+      </c>
+      <c r="D1857" t="n">
+        <v>19497</v>
+      </c>
+      <c r="E1857" t="n">
+        <v>19701.88</v>
+      </c>
+      <c r="F1857" t="n">
+        <v>19320.54</v>
+      </c>
+      <c r="G1857" t="n">
+        <v>22799</v>
+      </c>
+      <c r="H1857" t="n">
+        <v>19291.75</v>
+      </c>
+      <c r="I1857" t="n">
+        <v>21360.11</v>
+      </c>
+    </row>
+    <row r="1858">
+      <c r="A1858" s="2" t="n">
+        <v>44820</v>
+      </c>
+      <c r="B1858" t="n">
+        <v>19701.88</v>
+      </c>
+      <c r="C1858" t="n">
+        <v>19890</v>
+      </c>
+      <c r="D1858" t="n">
+        <v>19320.01</v>
+      </c>
+      <c r="E1858" t="n">
+        <v>19803.3</v>
+      </c>
+      <c r="F1858" t="n">
+        <v>21361.62</v>
+      </c>
+      <c r="G1858" t="n">
+        <v>22799</v>
+      </c>
+      <c r="H1858" t="n">
+        <v>19320.01</v>
+      </c>
+      <c r="I1858" t="n">
+        <v>21648.34</v>
+      </c>
+    </row>
+    <row r="1859">
+      <c r="A1859" s="2" t="n">
+        <v>44821</v>
+      </c>
+      <c r="B1859" t="n">
+        <v>19803.3</v>
+      </c>
+      <c r="C1859" t="n">
+        <v>20189</v>
+      </c>
+      <c r="D1859" t="n">
+        <v>19748.08</v>
+      </c>
+      <c r="E1859" t="n">
+        <v>20113.62</v>
+      </c>
+      <c r="F1859" t="n">
+        <v>21647.21</v>
+      </c>
+      <c r="G1859" t="n">
+        <v>22799</v>
+      </c>
+      <c r="H1859" t="n">
+        <v>19320.01</v>
+      </c>
+      <c r="I1859" t="n">
+        <v>21826.87</v>
+      </c>
+    </row>
+    <row r="1860">
+      <c r="A1860" s="2" t="n">
+        <v>44822</v>
+      </c>
+      <c r="B1860" t="n">
+        <v>20112.61</v>
+      </c>
+      <c r="C1860" t="n">
+        <v>20117.26</v>
+      </c>
+      <c r="D1860" t="n">
+        <v>19335.62</v>
+      </c>
+      <c r="E1860" t="n">
+        <v>19416.18</v>
+      </c>
+      <c r="F1860" t="n">
+        <v>21826.87</v>
+      </c>
+      <c r="G1860" t="n">
+        <v>22799</v>
+      </c>
+      <c r="H1860" t="n">
+        <v>19320.01</v>
+      </c>
+      <c r="I1860" t="n">
+        <v>22395.74</v>
+      </c>
+    </row>
+    <row r="1861">
+      <c r="A1861" s="2" t="n">
+        <v>44823</v>
+      </c>
+      <c r="B1861" t="n">
+        <v>19417.45</v>
+      </c>
+      <c r="C1861" t="n">
+        <v>19686.2</v>
+      </c>
+      <c r="D1861" t="n">
+        <v>18232.56</v>
+      </c>
+      <c r="E1861" t="n">
+        <v>19537.02</v>
+      </c>
+      <c r="F1861" t="n">
+        <v>22395.44</v>
+      </c>
+      <c r="G1861" t="n">
+        <v>22799</v>
+      </c>
+      <c r="H1861" t="n">
+        <v>18232.56</v>
+      </c>
+      <c r="I1861" t="n">
+        <v>20173.57</v>
+      </c>
+    </row>
+    <row r="1862">
+      <c r="A1862" s="2" t="n">
+        <v>44824</v>
+      </c>
+      <c r="B1862" t="n">
+        <v>19537.02</v>
+      </c>
+      <c r="C1862" t="n">
+        <v>19634.62</v>
+      </c>
+      <c r="D1862" t="n">
+        <v>18711.87</v>
+      </c>
+      <c r="E1862" t="n">
+        <v>18875</v>
+      </c>
+      <c r="F1862" t="n">
+        <v>20173.62</v>
+      </c>
+      <c r="G1862" t="n">
+        <v>20541.48</v>
+      </c>
+      <c r="H1862" t="n">
+        <v>18232.56</v>
+      </c>
+      <c r="I1862" t="n">
+        <v>20226.71</v>
+      </c>
+    </row>
+    <row r="1863">
+      <c r="A1863" s="2" t="n">
+        <v>44825</v>
+      </c>
+      <c r="B1863" t="n">
+        <v>18874.31</v>
+      </c>
+      <c r="C1863" t="n">
+        <v>19956</v>
+      </c>
+      <c r="D1863" t="n">
+        <v>18125.98</v>
+      </c>
+      <c r="E1863" t="n">
+        <v>18461.36</v>
+      </c>
+      <c r="F1863" t="n">
+        <v>20227.17</v>
+      </c>
+      <c r="G1863" t="n">
+        <v>20330.24</v>
+      </c>
+      <c r="H1863" t="n">
+        <v>18125.98</v>
+      </c>
+      <c r="I1863" t="n">
+        <v>19701.88</v>
+      </c>
+    </row>
+    <row r="1864">
+      <c r="A1864" s="2" t="n">
+        <v>44826</v>
+      </c>
+      <c r="B1864" t="n">
+        <v>18461.36</v>
+      </c>
+      <c r="C1864" t="n">
+        <v>19550.17</v>
+      </c>
+      <c r="D1864" t="n">
+        <v>18356.39</v>
+      </c>
+      <c r="E1864" t="n">
+        <v>19401.63</v>
+      </c>
+      <c r="F1864" t="n">
+        <v>19701.88</v>
+      </c>
+      <c r="G1864" t="n">
+        <v>20189</v>
+      </c>
+      <c r="H1864" t="n">
+        <v>18125.98</v>
+      </c>
+      <c r="I1864" t="n">
+        <v>19803.3</v>
+      </c>
+    </row>
+    <row r="1865">
+      <c r="A1865" s="2" t="n">
+        <v>44827</v>
+      </c>
+      <c r="B1865" t="n">
+        <v>19401.63</v>
+      </c>
+      <c r="C1865" t="n">
+        <v>19500</v>
+      </c>
+      <c r="D1865" t="n">
+        <v>18531.42</v>
+      </c>
+      <c r="E1865" t="n">
+        <v>19289.91</v>
+      </c>
+      <c r="F1865" t="n">
+        <v>19803.3</v>
+      </c>
+      <c r="G1865" t="n">
+        <v>20189</v>
+      </c>
+      <c r="H1865" t="n">
+        <v>18125.98</v>
+      </c>
+      <c r="I1865" t="n">
+        <v>20113.62</v>
+      </c>
+    </row>
+    <row r="1866">
+      <c r="A1866" s="2" t="n">
+        <v>44828</v>
+      </c>
+      <c r="B1866" t="n">
+        <v>19288.57</v>
+      </c>
+      <c r="C1866" t="n">
+        <v>19316.14</v>
+      </c>
+      <c r="D1866" t="n">
+        <v>18805.34</v>
+      </c>
+      <c r="E1866" t="n">
+        <v>18920.5</v>
+      </c>
+      <c r="F1866" t="n">
+        <v>20112.61</v>
+      </c>
+      <c r="G1866" t="n">
+        <v>20117.26</v>
+      </c>
+      <c r="H1866" t="n">
+        <v>18125.98</v>
+      </c>
+      <c r="I1866" t="n">
+        <v>19416.18</v>
+      </c>
+    </row>
+    <row r="1867">
+      <c r="A1867" s="2" t="n">
+        <v>44829</v>
+      </c>
+      <c r="B1867" t="n">
+        <v>18921.99</v>
+      </c>
+      <c r="C1867" t="n">
+        <v>19180.21</v>
+      </c>
+      <c r="D1867" t="n">
+        <v>18629.2</v>
+      </c>
+      <c r="E1867" t="n">
+        <v>18807.38</v>
+      </c>
+      <c r="F1867" t="n">
+        <v>19417.45</v>
+      </c>
+      <c r="G1867" t="n">
+        <v>19956</v>
+      </c>
+      <c r="H1867" t="n">
+        <v>18125.98</v>
+      </c>
+      <c r="I1867" t="n">
+        <v>19537.02</v>
+      </c>
+    </row>
+    <row r="1868">
+      <c r="A1868" s="2" t="n">
+        <v>44830</v>
+      </c>
+      <c r="B1868" t="n">
+        <v>18809.13</v>
+      </c>
+      <c r="C1868" t="n">
+        <v>19318.96</v>
+      </c>
+      <c r="D1868" t="n">
+        <v>18680.72</v>
+      </c>
+      <c r="E1868" t="n">
+        <v>19227.82</v>
+      </c>
+      <c r="F1868" t="n">
+        <v>19537.02</v>
+      </c>
+      <c r="G1868" t="n">
+        <v>19956</v>
+      </c>
+      <c r="H1868" t="n">
+        <v>18125.98</v>
+      </c>
+      <c r="I1868" t="n">
+        <v>18875</v>
+      </c>
+    </row>
+    <row r="1869">
+      <c r="A1869" s="2" t="n">
+        <v>44831</v>
+      </c>
+      <c r="B1869" t="n">
+        <v>19226.68</v>
+      </c>
+      <c r="C1869" t="n">
+        <v>20385.86</v>
+      </c>
+      <c r="D1869" t="n">
+        <v>18816.32</v>
+      </c>
+      <c r="E1869" t="n">
+        <v>19079.13</v>
+      </c>
+      <c r="F1869" t="n">
+        <v>18874.31</v>
+      </c>
+      <c r="G1869" t="n">
+        <v>20385.86</v>
+      </c>
+      <c r="H1869" t="n">
+        <v>18125.98</v>
+      </c>
+      <c r="I1869" t="n">
+        <v>18461.36</v>
+      </c>
+    </row>
+    <row r="1870">
+      <c r="A1870" s="2" t="n">
+        <v>44832</v>
+      </c>
+      <c r="B1870" t="n">
+        <v>19078.1</v>
+      </c>
+      <c r="C1870" t="n">
+        <v>19790</v>
+      </c>
+      <c r="D1870" t="n">
+        <v>18471.28</v>
+      </c>
+      <c r="E1870" t="n">
+        <v>19412.82</v>
+      </c>
+      <c r="F1870" t="n">
+        <v>18461.36</v>
+      </c>
+      <c r="G1870" t="n">
+        <v>20385.86</v>
+      </c>
+      <c r="H1870" t="n">
+        <v>18356.39</v>
+      </c>
+      <c r="I1870" t="n">
+        <v>19401.63</v>
+      </c>
+    </row>
+    <row r="1871">
+      <c r="A1871" s="2" t="n">
+        <v>44833</v>
+      </c>
+      <c r="B1871" t="n">
+        <v>19412.82</v>
+      </c>
+      <c r="C1871" t="n">
+        <v>19645.52</v>
+      </c>
+      <c r="D1871" t="n">
+        <v>18843.01</v>
+      </c>
+      <c r="E1871" t="n">
+        <v>19591.51</v>
+      </c>
+      <c r="F1871" t="n">
+        <v>19401.63</v>
+      </c>
+      <c r="G1871" t="n">
+        <v>20385.86</v>
+      </c>
+      <c r="H1871" t="n">
+        <v>18471.28</v>
+      </c>
+      <c r="I1871" t="n">
+        <v>19289.91</v>
+      </c>
+    </row>
+    <row r="1872">
+      <c r="A1872" s="2" t="n">
+        <v>44834</v>
+      </c>
+      <c r="B1872" t="n">
+        <v>19590.54</v>
+      </c>
+      <c r="C1872" t="n">
+        <v>20185</v>
+      </c>
+      <c r="D1872" t="n">
+        <v>19155.36</v>
+      </c>
+      <c r="E1872" t="n">
+        <v>19422.61</v>
+      </c>
+      <c r="F1872" t="n">
+        <v>19288.57</v>
+      </c>
+      <c r="G1872" t="n">
+        <v>20385.86</v>
+      </c>
+      <c r="H1872" t="n">
+        <v>18471.28</v>
+      </c>
+      <c r="I1872" t="n">
+        <v>18920.5</v>
+      </c>
+    </row>
+    <row r="1873">
+      <c r="A1873" s="2" t="n">
+        <v>44835</v>
+      </c>
+      <c r="B1873" t="n">
+        <v>19422.61</v>
+      </c>
+      <c r="C1873" t="n">
+        <v>19484</v>
+      </c>
+      <c r="D1873" t="n">
+        <v>19159.42</v>
+      </c>
+      <c r="E1873" t="n">
+        <v>19310.95</v>
+      </c>
+      <c r="F1873" t="n">
+        <v>18921.99</v>
+      </c>
+      <c r="G1873" t="n">
+        <v>20385.86</v>
+      </c>
+      <c r="H1873" t="n">
+        <v>18471.28</v>
+      </c>
+      <c r="I1873" t="n">
+        <v>18807.38</v>
+      </c>
+    </row>
+    <row r="1874">
+      <c r="A1874" s="2" t="n">
+        <v>44836</v>
+      </c>
+      <c r="B1874" t="n">
+        <v>19312.24</v>
+      </c>
+      <c r="C1874" t="n">
+        <v>19395.91</v>
+      </c>
+      <c r="D1874" t="n">
+        <v>18920.35</v>
+      </c>
+      <c r="E1874" t="n">
+        <v>19056.8</v>
+      </c>
+      <c r="F1874" t="n">
+        <v>18809.13</v>
+      </c>
+      <c r="G1874" t="n">
+        <v>20385.86</v>
+      </c>
+      <c r="H1874" t="n">
+        <v>18471.28</v>
+      </c>
+      <c r="I1874" t="n">
+        <v>19227.82</v>
+      </c>
+    </row>
+    <row r="1875">
+      <c r="A1875" s="2" t="n">
+        <v>44837</v>
+      </c>
+      <c r="B1875" t="n">
+        <v>19057.74</v>
+      </c>
+      <c r="C1875" t="n">
+        <v>19719.1</v>
+      </c>
+      <c r="D1875" t="n">
+        <v>18959.68</v>
+      </c>
+      <c r="E1875" t="n">
+        <v>19629.08</v>
+      </c>
+      <c r="F1875" t="n">
+        <v>19226.68</v>
+      </c>
+      <c r="G1875" t="n">
+        <v>20385.86</v>
+      </c>
+      <c r="H1875" t="n">
+        <v>18471.28</v>
+      </c>
+      <c r="I1875" t="n">
+        <v>19079.13</v>
+      </c>
+    </row>
+    <row r="1876">
+      <c r="A1876" s="2" t="n">
+        <v>44838</v>
+      </c>
+      <c r="B1876" t="n">
+        <v>19629.08</v>
+      </c>
+      <c r="C1876" t="n">
+        <v>20475</v>
+      </c>
+      <c r="D1876" t="n">
+        <v>19490.6</v>
+      </c>
+      <c r="E1876" t="n">
+        <v>20337.82</v>
+      </c>
+      <c r="F1876" t="n">
+        <v>19078.1</v>
+      </c>
+      <c r="G1876" t="n">
+        <v>20475</v>
+      </c>
+      <c r="H1876" t="n">
+        <v>18471.28</v>
+      </c>
+      <c r="I1876" t="n">
+        <v>19412.82</v>
+      </c>
+    </row>
+    <row r="1877">
+      <c r="A1877" s="2" t="n">
+        <v>44839</v>
+      </c>
+      <c r="B1877" t="n">
+        <v>20337.82</v>
+      </c>
+      <c r="C1877" t="n">
+        <v>20365.6</v>
+      </c>
+      <c r="D1877" t="n">
+        <v>19730</v>
+      </c>
+      <c r="E1877" t="n">
+        <v>20158.26</v>
+      </c>
+      <c r="F1877" t="n">
+        <v>19412.82</v>
+      </c>
+      <c r="G1877" t="n">
+        <v>20475</v>
+      </c>
+      <c r="H1877" t="n">
+        <v>18843.01</v>
+      </c>
+      <c r="I1877" t="n">
+        <v>19591.51</v>
+      </c>
+    </row>
+    <row r="1878">
+      <c r="A1878" s="2" t="n">
+        <v>44840</v>
+      </c>
+      <c r="B1878" t="n">
+        <v>20158.26</v>
+      </c>
+      <c r="C1878" t="n">
+        <v>20456.6</v>
+      </c>
+      <c r="D1878" t="n">
+        <v>19853</v>
+      </c>
+      <c r="E1878" t="n">
+        <v>19960.67</v>
+      </c>
+      <c r="F1878" t="n">
+        <v>19590.54</v>
+      </c>
+      <c r="G1878" t="n">
+        <v>20475</v>
+      </c>
+      <c r="H1878" t="n">
+        <v>18920.35</v>
+      </c>
+      <c r="I1878" t="n">
+        <v>19422.61</v>
+      </c>
+    </row>
+    <row r="1879">
+      <c r="A1879" s="2" t="n">
+        <v>44841</v>
+      </c>
+      <c r="B1879" t="n">
+        <v>19960.67</v>
+      </c>
+      <c r="C1879" t="n">
+        <v>20068.82</v>
+      </c>
+      <c r="D1879" t="n">
+        <v>19320</v>
+      </c>
+      <c r="E1879" t="n">
+        <v>19530.09</v>
+      </c>
+      <c r="F1879" t="n">
+        <v>19422.61</v>
+      </c>
+      <c r="G1879" t="n">
+        <v>20475</v>
+      </c>
+      <c r="H1879" t="n">
+        <v>18920.35</v>
+      </c>
+      <c r="I1879" t="n">
+        <v>19310.95</v>
+      </c>
+    </row>
+    <row r="1880">
+      <c r="A1880" s="2" t="n">
+        <v>44842</v>
+      </c>
+      <c r="B1880" t="n">
+        <v>19530.09</v>
+      </c>
+      <c r="C1880" t="n">
+        <v>19627.38</v>
+      </c>
+      <c r="D1880" t="n">
+        <v>19237.14</v>
+      </c>
+      <c r="E1880" t="n">
+        <v>19417.96</v>
+      </c>
+      <c r="F1880" t="n">
+        <v>19312.24</v>
+      </c>
+      <c r="G1880" t="n">
+        <v>20475</v>
+      </c>
+      <c r="H1880" t="n">
+        <v>18920.35</v>
+      </c>
+      <c r="I1880" t="n">
+        <v>19056.8</v>
+      </c>
+    </row>
+    <row r="1881">
+      <c r="A1881" s="2" t="n">
+        <v>44843</v>
+      </c>
+      <c r="B1881" t="n">
+        <v>19416.52</v>
+      </c>
+      <c r="C1881" t="n">
+        <v>19558</v>
+      </c>
+      <c r="D1881" t="n">
+        <v>19316.04</v>
+      </c>
+      <c r="E1881" t="n">
+        <v>19439.02</v>
+      </c>
+      <c r="F1881" t="n">
+        <v>19057.74</v>
+      </c>
+      <c r="G1881" t="n">
+        <v>20475</v>
+      </c>
+      <c r="H1881" t="n">
+        <v>18959.68</v>
+      </c>
+      <c r="I1881" t="n">
+        <v>19629.08</v>
+      </c>
+    </row>
+    <row r="1882">
+      <c r="A1882" s="2" t="n">
+        <v>44844</v>
+      </c>
+      <c r="B1882" t="n">
+        <v>19439.96</v>
+      </c>
+      <c r="C1882" t="n">
+        <v>19525</v>
+      </c>
+      <c r="D1882" t="n">
+        <v>19020.25</v>
+      </c>
+      <c r="E1882" t="n">
+        <v>19131.87</v>
+      </c>
+      <c r="F1882" t="n">
+        <v>19629.08</v>
+      </c>
+      <c r="G1882" t="n">
+        <v>20475</v>
+      </c>
+      <c r="H1882" t="n">
+        <v>19020.25</v>
+      </c>
+      <c r="I1882" t="n">
+        <v>20337.82</v>
+      </c>
+    </row>
+    <row r="1883">
+      <c r="A1883" s="2" t="n">
+        <v>44845</v>
+      </c>
+      <c r="B1883" t="n">
+        <v>19131.87</v>
+      </c>
+      <c r="C1883" t="n">
+        <v>19268.09</v>
+      </c>
+      <c r="D1883" t="n">
+        <v>18860</v>
+      </c>
+      <c r="E1883" t="n">
+        <v>19060</v>
+      </c>
+      <c r="F1883" t="n">
+        <v>20337.82</v>
+      </c>
+      <c r="G1883" t="n">
+        <v>20456.6</v>
+      </c>
+      <c r="H1883" t="n">
+        <v>18860</v>
+      </c>
+      <c r="I1883" t="n">
+        <v>20158.26</v>
+      </c>
+    </row>
+    <row r="1884">
+      <c r="A1884" s="2" t="n">
+        <v>44846</v>
+      </c>
+      <c r="B1884" t="n">
+        <v>19060</v>
+      </c>
+      <c r="C1884" t="n">
+        <v>19238.31</v>
+      </c>
+      <c r="D1884" t="n">
+        <v>18965.88</v>
+      </c>
+      <c r="E1884" t="n">
+        <v>19155.53</v>
+      </c>
+      <c r="F1884" t="n">
+        <v>20158.26</v>
+      </c>
+      <c r="G1884" t="n">
+        <v>20456.6</v>
+      </c>
+      <c r="H1884" t="n">
+        <v>18860</v>
+      </c>
+      <c r="I1884" t="n">
+        <v>19960.67</v>
+      </c>
+    </row>
+    <row r="1885">
+      <c r="A1885" s="2" t="n">
+        <v>44847</v>
+      </c>
+      <c r="B1885" t="n">
+        <v>19155.1</v>
+      </c>
+      <c r="C1885" t="n">
+        <v>19513.79</v>
+      </c>
+      <c r="D1885" t="n">
+        <v>18190</v>
+      </c>
+      <c r="E1885" t="n">
+        <v>19375.13</v>
+      </c>
+      <c r="F1885" t="n">
+        <v>19960.67</v>
+      </c>
+      <c r="G1885" t="n">
+        <v>20068.82</v>
+      </c>
+      <c r="H1885" t="n">
+        <v>18190</v>
+      </c>
+      <c r="I1885" t="n">
+        <v>19530.09</v>
+      </c>
+    </row>
+    <row r="1886">
+      <c r="A1886" s="2" t="n">
+        <v>44848</v>
+      </c>
+      <c r="B1886" t="n">
+        <v>19375.58</v>
+      </c>
+      <c r="C1886" t="n">
+        <v>19951.87</v>
+      </c>
+      <c r="D1886" t="n">
+        <v>19100.01</v>
+      </c>
+      <c r="E1886" t="n">
+        <v>19176.41</v>
+      </c>
+      <c r="F1886" t="n">
+        <v>19530.09</v>
+      </c>
+      <c r="G1886" t="n">
+        <v>19951.87</v>
+      </c>
+      <c r="H1886" t="n">
+        <v>18190</v>
+      </c>
+      <c r="I1886" t="n">
+        <v>19417.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>